<commit_message>
modifications to step 2., step 3. and step 4. because of full dataset availability
</commit_message>
<xml_diff>
--- a/similarity_table_abst.xlsx
+++ b/similarity_table_abst.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Mean of similarity</t>
   </si>
@@ -31,28 +31,19 @@
     <t>Computed Tomography (ct)</t>
   </si>
   <si>
-    <t>Emergency Radiology (er)</t>
-  </si>
-  <si>
-    <t>Biomarkers and Quantative imaging (bq)</t>
-  </si>
-  <si>
-    <t>Safety and Quality (sq)</t>
-  </si>
-  <si>
-    <t>Professionalism (pr)</t>
-  </si>
-  <si>
-    <t>Nuclear Medicine (nm)</t>
+    <t>Breast Imaging (br)</t>
+  </si>
+  <si>
+    <t>Geritourinary Radiology (gu)</t>
+  </si>
+  <si>
+    <t>Ultrasound (us)</t>
   </si>
   <si>
     <t>Chest Radiology (ch)</t>
   </si>
   <si>
-    <t>Breast Imaging (br)</t>
-  </si>
-  <si>
-    <t>Geritourinary Radiology (gu)</t>
+    <t>Interventional Radiology (ir)</t>
   </si>
 </sst>
 </file>
@@ -384,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,13 +397,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.003537936797399456</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.02166382793468516</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -426,7 +417,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -434,13 +425,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.01704682499148335</v>
+        <v>0.1432560135011233</v>
       </c>
       <c r="C4">
-        <v>0.03225477005173821</v>
+        <v>0.1084180057565769</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -448,13 +439,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.06003377183773705</v>
+        <v>0.0009685406801488272</v>
       </c>
       <c r="C5">
-        <v>0.06097882980865835</v>
+        <v>0.009588063559035733</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -462,13 +453,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.02195124199999536</v>
+        <v>0.005598125815857243</v>
       </c>
       <c r="C6">
-        <v>0.0423017720018925</v>
+        <v>0.02730579349881621</v>
       </c>
       <c r="D6">
-        <v>9</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -476,13 +467,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.01240836581265891</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.02990742360884703</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -490,55 +481,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.005393984377847852</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.0274330692286452</v>
       </c>
       <c r="D8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0.03073320708217532</v>
-      </c>
-      <c r="C9">
-        <v>0.04371723153638751</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>0.1242335733303064</v>
-      </c>
-      <c r="C10">
-        <v>0.08333330862754358</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use preprocessed data instead of raw
</commit_message>
<xml_diff>
--- a/similarity_table_abst.xlsx
+++ b/similarity_table_abst.xlsx
@@ -397,10 +397,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.003537936797399456</v>
+        <v>0.00367626090550077</v>
       </c>
       <c r="C2">
-        <v>0.02166382793468516</v>
+        <v>0.0226341828951084</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -425,10 +425,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1432560135011233</v>
+        <v>0.1554389076685921</v>
       </c>
       <c r="C4">
-        <v>0.1084180057565769</v>
+        <v>0.1160159412858153</v>
       </c>
       <c r="D4">
         <v>98</v>
@@ -453,10 +453,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.005598125815857243</v>
+        <v>0.005762297447160056</v>
       </c>
       <c r="C6">
-        <v>0.02730579349881621</v>
+        <v>0.02806713873169302</v>
       </c>
       <c r="D6">
         <v>96</v>
@@ -467,10 +467,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.01240836581265891</v>
+        <v>0.01339957145108256</v>
       </c>
       <c r="C7">
-        <v>0.02990742360884703</v>
+        <v>0.03246039764789236</v>
       </c>
       <c r="D7">
         <v>99</v>
@@ -481,10 +481,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.005393984377847852</v>
+        <v>0.005619484334682075</v>
       </c>
       <c r="C8">
-        <v>0.0274330692286452</v>
+        <v>0.02826951386241152</v>
       </c>
       <c r="D8">
         <v>96</v>

</xml_diff>